<commit_message>
clean up _bdn foldere
</commit_message>
<xml_diff>
--- a/_dat/cost/Copy of PSPAP_historic funding_for Mike Colvin.xlsx
+++ b/_dat/cost/Copy of PSPAP_historic funding_for Mike Colvin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16608" windowHeight="9432" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16392" windowHeight="5304" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PSPAP History" sheetId="1" r:id="rId1"/>
@@ -713,7 +713,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1250,7 +1250,7 @@
   <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>